<commit_message>
Màj des exemples ODS et XSLX
</commit_message>
<xml_diff>
--- a/exemples/exemple-valide.xlsx
+++ b/exemples/exemple-valide.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="51">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -82,6 +82,9 @@
     <t xml:space="preserve">objetModification</t>
   </si>
   <si>
+    <t xml:space="preserve">source</t>
+  </si>
+  <si>
     <t xml:space="preserve">donneesActuelles</t>
   </si>
   <si>
@@ -142,6 +145,12 @@
     <t xml:space="preserve">Colin Maudry</t>
   </si>
   <si>
+    <t xml:space="preserve">data.gouv.fr_aife</t>
+  </si>
+  <si>
+    <t xml:space="preserve">non</t>
+  </si>
+  <si>
     <t xml:space="preserve">82379887100013</t>
   </si>
   <si>
@@ -161,6 +170,9 @@
   </si>
   <si>
     <t xml:space="preserve">Augmentation de la durée du marché à 6 mois.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oui</t>
   </si>
 </sst>
 </file>
@@ -261,7 +273,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V5"/>
+  <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -289,8 +301,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="19.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="24.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="39.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="15.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="9.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="14.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="9.77"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -360,259 +373,274 @@
       <c r="V1" s="0" t="s">
         <v>21</v>
       </c>
+      <c r="W1" s="0" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L2" s="0" t="n">
         <v>3</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="U2" s="0" t="n">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="U2" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="V2" s="0" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L3" s="0" t="n">
         <v>3</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="R3" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="S3" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="U3" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="U3" s="0" t="n">
-        <v>0</v>
+      <c r="V3" s="0" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L4" s="0" t="n">
         <v>6</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P4" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="R4" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="S4" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="T4" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="U4" s="0" t="n">
-        <v>1</v>
+        <v>49</v>
+      </c>
+      <c r="U4" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="V4" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L5" s="0" t="n">
         <v>6</v>
       </c>
       <c r="M5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O5" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="P5" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R5" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="S5" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="N5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="O5" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="P5" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="R5" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="S5" s="0" t="s">
+      <c r="T5" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="U5" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="T5" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="U5" s="0" t="n">
-        <v>1</v>
+      <c r="V5" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>